<commit_message>
Created Flask_attempt python file, to try uploading zip files without saving on local drive.
</commit_message>
<xml_diff>
--- a/Generated_Data.xlsx
+++ b/Generated_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>index</t>
   </si>
@@ -43,28 +43,40 @@
     <t>2133-3d-massing-BenoyPA</t>
   </si>
   <si>
-    <t>W23</t>
-  </si>
-  <si>
-    <t>W29</t>
-  </si>
-  <si>
-    <t>W24</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
-    <t>F2</t>
+    <t>2133-3d-massing-PP-opt2</t>
+  </si>
+  <si>
+    <t>2133-3d-massing-PP-opt1</t>
+  </si>
+  <si>
+    <t>W25</t>
+  </si>
+  <si>
+    <t>W316</t>
+  </si>
+  <si>
+    <t>W313</t>
+  </si>
+  <si>
+    <t>W7</t>
   </si>
   <si>
     <t>F0</t>
   </si>
   <si>
-    <t>59°N</t>
+    <t>SWAF0</t>
+  </si>
+  <si>
+    <t>SWAF2</t>
+  </si>
+  <si>
+    <t>SWAF1</t>
   </si>
   <si>
     <t>60°N</t>
+  </si>
+  <si>
+    <t>147°</t>
   </si>
 </sst>
 </file>
@@ -154,7 +166,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="VSC-_F3_W230.Jpeg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="VSC-_F0_W25.Jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -192,7 +204,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="VSC-_F0_W292.Jpeg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="VSC-_F0_W316.Jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -230,7 +242,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="VSC-_F0_W24.Jpeg"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="VSC-_F2_W313.Jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -268,13 +280,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="VSC-_F3_W230.Jpeg"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="VSC-_F0_W70.Jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -625,22 +637,22 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>17.1</v>
+        <v>24.3</v>
       </c>
       <c r="F2">
-        <v>4.2</v>
+        <v>10.1</v>
       </c>
       <c r="G2">
-        <v>0.25</v>
+        <v>0.42</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="110" customHeight="1">
@@ -648,25 +660,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3">
-        <v>27.5</v>
+        <v>21</v>
       </c>
       <c r="F3">
-        <v>11.2</v>
+        <v>18.7</v>
       </c>
       <c r="G3">
-        <v>0.41</v>
+        <v>0.89</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="110" customHeight="1">
@@ -674,25 +686,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4">
-        <v>23.6</v>
+        <v>28.6</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G4">
-        <v>0.38</v>
+        <v>0.73</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="110" customHeight="1">
@@ -700,25 +712,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E5">
-        <v>17.1</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>4.2</v>
+        <v>18.2</v>
       </c>
       <c r="G5">
-        <v>0.25</v>
+        <v>0.73</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>